<commit_message>
+ SUBX and fix ADDX bug
</commit_message>
<xml_diff>
--- a/instruction set.xlsx
+++ b/instruction set.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
   <si>
     <t>instruction</t>
   </si>
@@ -127,6 +127,15 @@
   </si>
   <si>
     <t>011</t>
+  </si>
+  <si>
+    <t>SUBX;a-x-&gt;a</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>0010010</t>
   </si>
 </sst>
 </file>
@@ -504,7 +513,7 @@
   <dimension ref="A1:R53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,20 +845,68 @@
         <v>21</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="Q6" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>1010000101000000000</v>
+        <v>1010000101010000000</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="Q7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>1010000101010010010</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">

</xml_diff>